<commit_message>
mise à jour para eliminar de Inedit Sharepoint
</commit_message>
<xml_diff>
--- a/docs/www/data/II/1-In-depth analysis-UNIN.xlsx
+++ b/docs/www/data/II/1-In-depth analysis-UNIN.xlsx
@@ -6860,9 +6860,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE2C641D63AAEB479C875906D47D0865" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="ab436c20fa8d39dcae98f89eebf39103">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7cd0a2e4-f300-47b4-9e62-47e720d2debb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="657358c3c105dec4c76f5913543d781c" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE2C641D63AAEB479C875906D47D0865" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="075bcab0c05fd268fca7f6a5657dc319">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7cd0a2e4-f300-47b4-9e62-47e720d2debb" xmlns:ns3="f2a4cf12-9b78-416c-99ba-8a93f354c4ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7c92028e921235b861245ee9ccfde2a" ns2:_="" ns3:_="">
     <xsd:import namespace="7cd0a2e4-f300-47b4-9e62-47e720d2debb"/>
+    <xsd:import namespace="f2a4cf12-9b78-416c-99ba-8a93f354c4ba"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -6877,6 +6878,10 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6929,6 +6934,46 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f2a4cf12-9b78-416c-99ba-8a93f354c4ba" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7047,7 +7092,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE87D082-0479-4444-A00F-949CD55DE57F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61291FC0-5945-428E-A3BB-1F61089875D7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>